<commit_message>
Funktion som returnerar array med 4 slumptal 0-7
</commit_message>
<xml_diff>
--- a/Dokument/Iterationsplan.xlsx
+++ b/Dokument/Iterationsplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Iterationsplan v 14</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Påbörjat</t>
+  </si>
+  <si>
+    <t>Färdig</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -656,9 +659,12 @@
         <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extra uppgifter tillagda för iteration 0
</commit_message>
<xml_diff>
--- a/Dokument/Iterationsplan.xlsx
+++ b/Dokument/Iterationsplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Iterationsplan v 14</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Färdig</t>
+  </si>
+  <si>
+    <t>Skapa metod för introduktionstext</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D22" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,7 +627,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -641,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>17</v>
@@ -654,7 +657,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -668,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -682,50 +685,60 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" t="s">
         <v>19</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4">
-        <v>5</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" t="s">
-        <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="4">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="4">
         <v>3</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="D29" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lade till de olika symbolerna som används som pjäser
</commit_message>
<xml_diff>
--- a/Dokument/Iterationsplan.xlsx
+++ b/Dokument/Iterationsplan.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Iterationsplan v 14</t>
-  </si>
-  <si>
-    <t>-1, Uppstart</t>
   </si>
   <si>
     <t>Introduktionsföreläsning</t>
@@ -474,17 +471,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
@@ -496,29 +493,29 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
+      <c r="A5" s="3">
+        <v>-1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
         <v>2</v>
@@ -530,7 +527,7 @@
     <row r="6" spans="1:4">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -542,7 +539,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -554,7 +551,7 @@
     <row r="8" spans="1:4">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="6">
         <v>3</v>
@@ -566,7 +563,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -578,7 +575,7 @@
     <row r="10" spans="1:4">
       <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -590,7 +587,7 @@
     <row r="11" spans="1:4">
       <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5">
@@ -600,7 +597,7 @@
     <row r="12" spans="1:4">
       <c r="A12" s="5"/>
       <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -619,135 +616,145 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>0</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="4">
-        <v>3</v>
+      <c r="D18" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E18" s="4">
         <v>3</v>
       </c>
+      <c r="F18" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="4">
-        <v>2</v>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E21" s="4">
         <v>2</v>
       </c>
+      <c r="F21" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="C23" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4">
-        <v>5</v>
-      </c>
-      <c r="E22" s="4">
-        <v>9</v>
-      </c>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="D23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="4">
         <v>3</v>
       </c>
-      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="D24" s="4"/>
-      <c r="E24" s="7">
+      <c r="E24" s="4"/>
+      <c r="F24" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:6">
+      <c r="A25" s="1"/>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:6">
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:6">
+      <c r="A27" s="1"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:6">
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:6">
+      <c r="A29" s="1"/>
       <c r="D29" s="4"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>